<commit_message>
improve linkedin brower automation
</commit_message>
<xml_diff>
--- a/inb/linkedin-data.xlsx
+++ b/inb/linkedin-data.xlsx
@@ -873,8 +873,16 @@
           <t>Spotnana</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>no_connect_button</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -892,8 +900,16 @@
           <t>MX Player</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>no_connect_button</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">

</xml_diff>